<commit_message>
ädd solfl part 1
</commit_message>
<xml_diff>
--- a/data/Web3 wallets.xlsx
+++ b/data/Web3 wallets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacks\Web3-Portfolio-Analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86E8303-6AFB-46E2-A7E4-E75CA8516E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4C208D-F7AE-4B8F-8DCA-D05573AE8FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-910" windowWidth="38620" windowHeight="21100" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="86280" yWindow="8565" windowWidth="20640" windowHeight="11040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>

</xml_diff>